<commit_message>
Regione: REGIONE_LAZIO, Issuer: integrity:S1#VILAZIO
</commit_message>
<xml_diff>
--- a/REGIONE_LAZIO/integrity:S1#VILAZIO.xlsx
+++ b/REGIONE_LAZIO/integrity:S1#VILAZIO.xlsx
@@ -41,13 +41,13 @@
     <t>NGNVCN92S19L259C^^^&amp;2.16.840.1.113883.2.9.4.3.2&amp;ISO</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.e7e6b389db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.be7ba7c0c7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721645763907</t>
+    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721646186259</t>
   </si>
   <si>
-    <t>22-07-2024:12:56:06</t>
+    <t>22-07-2024:13:03:07</t>
   </si>
   <si>
     <t>Creazione_0</t>
@@ -56,13 +56,13 @@
     <t>MRCLSN97C14H501J^^^&amp;2.16.840.1.113883.2.9.4.3.2&amp;ISO</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.dc1d06ac10^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.1a94c8365b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721645752195</t>
+    <t>2.16.840.1.113883.2.9.2.110.4.4^UAT_GTW_ID1721646174009</t>
   </si>
   <si>
-    <t>22-07-2024:12:55:54</t>
+    <t>22-07-2024:13:02:56</t>
   </si>
 </sst>
 </file>

</xml_diff>